<commit_message>
Successful multiple document transformation
</commit_message>
<xml_diff>
--- a/Merged SPO reports/merged_spo_06-09-23.xlsx
+++ b/Merged SPO reports/merged_spo_06-09-23.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,79 +626,75 @@
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Makayla Baca</t>
+          <t>Aminah Avalos</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+        <v>11</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.5</v>
       </c>
       <c r="F3" t="n">
-        <v>3852.42</v>
+        <v>3067</v>
       </c>
       <c r="G3" t="n">
-        <v>4148.77</v>
+        <v>3304.76</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>16.16</v>
       </c>
       <c r="J3" t="n">
-        <v>28</v>
+        <v>51.5</v>
       </c>
       <c r="K3" t="n">
-        <v>30.16</v>
+        <v>55.5</v>
       </c>
       <c r="L3" t="n">
-        <v>3880.42</v>
+        <v>3133.5</v>
       </c>
       <c r="M3" t="n">
-        <v>4178.93</v>
+        <v>3376.42</v>
       </c>
       <c r="N3" t="n">
-        <v>80.84</v>
+        <v>74.60714285714286</v>
       </c>
       <c r="O3" t="n">
-        <v>87.06</v>
+        <v>80.39095238095238</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Vy Torino</t>
+          <t>Celeste Perez (A)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+        <v>11</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.2</v>
       </c>
       <c r="F4" t="n">
-        <v>2815.3</v>
+        <v>1965.5</v>
       </c>
       <c r="G4" t="n">
-        <v>3031.7</v>
+        <v>2117.87</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -707,49 +703,47 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>5.38</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>2820.3</v>
+        <v>1965.5</v>
       </c>
       <c r="M4" t="n">
-        <v>3037.08</v>
+        <v>2117.87</v>
       </c>
       <c r="N4" t="n">
-        <v>76.22</v>
+        <v>75.59615384615384</v>
       </c>
       <c r="O4" t="n">
-        <v>82.08</v>
+        <v>81.45653846153846</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Justyne Martinez </t>
+          <t>Danielle Mai</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>2149.7</v>
+        <v>484.9</v>
       </c>
       <c r="G5" t="n">
-        <v>2315.43</v>
+        <v>522.17</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -758,49 +752,47 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>21.54</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>2169.7</v>
+        <v>484.9</v>
       </c>
       <c r="M5" t="n">
-        <v>2336.97</v>
+        <v>522.17</v>
       </c>
       <c r="N5" t="n">
-        <v>67.8</v>
+        <v>80.81666666666666</v>
       </c>
       <c r="O5" t="n">
-        <v>73.03</v>
+        <v>87.02833333333332</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Maggie  Farrell</t>
+          <t>Izzy Kruis</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.5</v>
       </c>
       <c r="F6" t="n">
-        <v>1740.3</v>
+        <v>2889.6</v>
       </c>
       <c r="G6" t="n">
-        <v>1874.05</v>
+        <v>3113.63</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -809,49 +801,47 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>49.53</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1786.3</v>
+        <v>2889.6</v>
       </c>
       <c r="M6" t="n">
-        <v>1923.58</v>
+        <v>3113.63</v>
       </c>
       <c r="N6" t="n">
-        <v>68.7</v>
+        <v>62.81739130434782</v>
       </c>
       <c r="O6" t="n">
-        <v>73.98</v>
+        <v>67.68760869565217</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Danielle Mai</t>
+          <t>Jasmine Saiz</t>
         </is>
       </c>
       <c r="B7" t="n">
+        <v>37</v>
+      </c>
+      <c r="C7" t="n">
+        <v>19</v>
+      </c>
+      <c r="D7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E7" t="n">
+        <v>2.5</v>
       </c>
       <c r="F7" t="n">
-        <v>484.9</v>
+        <v>2391.46</v>
       </c>
       <c r="G7" t="n">
-        <v>522.17</v>
+        <v>2577.18</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -860,100 +850,96 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>22.09</v>
       </c>
       <c r="L7" t="n">
-        <v>484.9</v>
+        <v>2411.96</v>
       </c>
       <c r="M7" t="n">
-        <v>522.17</v>
+        <v>2599.27</v>
       </c>
       <c r="N7" t="n">
-        <v>80.81999999999999</v>
+        <v>65.18810810810811</v>
       </c>
       <c r="O7" t="n">
-        <v>87.03</v>
+        <v>70.25054054054054</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Aminah Avalos</t>
+          <t xml:space="preserve">Justyne Martinez </t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D8" t="n">
-        <v>11</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2.5</v>
       </c>
       <c r="F8" t="n">
-        <v>3067</v>
+        <v>2149.7</v>
       </c>
       <c r="G8" t="n">
-        <v>3304.76</v>
+        <v>2315.43</v>
       </c>
       <c r="H8" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>16.16</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>51.5</v>
+        <v>20</v>
       </c>
       <c r="K8" t="n">
-        <v>55.5</v>
+        <v>21.54</v>
       </c>
       <c r="L8" t="n">
-        <v>3133.5</v>
+        <v>2169.7</v>
       </c>
       <c r="M8" t="n">
-        <v>3376.42</v>
+        <v>2336.97</v>
       </c>
       <c r="N8" t="n">
-        <v>74.61</v>
+        <v>67.80312499999999</v>
       </c>
       <c r="O8" t="n">
-        <v>80.39</v>
+        <v>73.03031249999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Izzy Kruis</t>
+          <t>Karen Trevizo</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C9" t="n">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4.6</v>
       </c>
       <c r="F9" t="n">
-        <v>2889.6</v>
+        <v>1508.7</v>
       </c>
       <c r="G9" t="n">
-        <v>3113.63</v>
+        <v>1624.88</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -968,43 +954,41 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>2889.6</v>
+        <v>1508.7</v>
       </c>
       <c r="M9" t="n">
-        <v>3113.63</v>
+        <v>1624.88</v>
       </c>
       <c r="N9" t="n">
-        <v>62.82</v>
+        <v>68.57727272727271</v>
       </c>
       <c r="O9" t="n">
-        <v>67.69</v>
+        <v>73.85818181818182</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Jasmine Saiz</t>
+          <t>Krisdee Martinez</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C10" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.5</v>
       </c>
       <c r="F10" t="n">
-        <v>2391.46</v>
+        <v>2141.25</v>
       </c>
       <c r="G10" t="n">
-        <v>2577.18</v>
+        <v>2307.68</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1013,49 +997,47 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>20.5</v>
+        <v>5</v>
       </c>
       <c r="K10" t="n">
-        <v>22.09</v>
+        <v>5.39</v>
       </c>
       <c r="L10" t="n">
-        <v>2411.96</v>
+        <v>2146.25</v>
       </c>
       <c r="M10" t="n">
-        <v>2599.27</v>
+        <v>2313.07</v>
       </c>
       <c r="N10" t="n">
-        <v>65.19</v>
+        <v>71.54166666666667</v>
       </c>
       <c r="O10" t="n">
-        <v>70.25</v>
+        <v>77.10233333333333</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Krisdee Martinez</t>
+          <t>Maggie  Farrell</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
         <v>3</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="E11" t="n">
+        <v>2.3</v>
       </c>
       <c r="F11" t="n">
-        <v>2141.25</v>
+        <v>1740.3</v>
       </c>
       <c r="G11" t="n">
-        <v>2307.68</v>
+        <v>1874.05</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1064,49 +1046,47 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="K11" t="n">
-        <v>5.39</v>
+        <v>49.53</v>
       </c>
       <c r="L11" t="n">
-        <v>2146.25</v>
+        <v>1786.3</v>
       </c>
       <c r="M11" t="n">
-        <v>2313.07</v>
+        <v>1923.58</v>
       </c>
       <c r="N11" t="n">
-        <v>71.54000000000001</v>
+        <v>68.70384615384616</v>
       </c>
       <c r="O11" t="n">
-        <v>77.09999999999999</v>
+        <v>73.98384615384614</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Celeste Perez (A)</t>
+          <t>Makayla Baca</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C12" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" t="n">
         <v>6</v>
       </c>
-      <c r="D12" t="n">
-        <v>11</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>4.4</t>
-        </is>
+      <c r="E12" t="n">
+        <v>2.5</v>
       </c>
       <c r="F12" t="n">
-        <v>1965.5</v>
+        <v>3852.42</v>
       </c>
       <c r="G12" t="n">
-        <v>2117.87</v>
+        <v>4148.77</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1115,560 +1095,70 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>30.16</v>
       </c>
       <c r="L12" t="n">
-        <v>1965.5</v>
+        <v>3880.42</v>
       </c>
       <c r="M12" t="n">
-        <v>2117.87</v>
+        <v>4178.93</v>
       </c>
       <c r="N12" t="n">
-        <v>75.59999999999999</v>
+        <v>80.84208333333333</v>
       </c>
       <c r="O12" t="n">
-        <v>81.45999999999999</v>
+        <v>87.06104166666667</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Aminah Avalos</t>
+          <t>Vy Torino</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C13" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D13" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13" t="n">
         <v>2.5</v>
       </c>
       <c r="F13" t="n">
-        <v>3067</v>
+        <v>2815.3</v>
       </c>
       <c r="G13" t="n">
-        <v>3304.76</v>
+        <v>3031.7</v>
       </c>
       <c r="H13" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>16.16</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>51.5</v>
+        <v>5</v>
       </c>
       <c r="K13" t="n">
-        <v>55.5</v>
+        <v>5.38</v>
       </c>
       <c r="L13" t="n">
-        <v>3133.5</v>
+        <v>2820.3</v>
       </c>
       <c r="M13" t="n">
-        <v>3376.42</v>
+        <v>3037.08</v>
       </c>
       <c r="N13" t="n">
-        <v>74.60714285714286</v>
+        <v>76.22432432432433</v>
       </c>
       <c r="O13" t="n">
-        <v>80.39095238095238</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Celeste Perez (A)</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>26</v>
-      </c>
-      <c r="C14" t="n">
-        <v>6</v>
-      </c>
-      <c r="D14" t="n">
-        <v>11</v>
-      </c>
-      <c r="E14" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1965.5</v>
-      </c>
-      <c r="G14" t="n">
-        <v>2117.87</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>1965.5</v>
-      </c>
-      <c r="M14" t="n">
-        <v>2117.87</v>
-      </c>
-      <c r="N14" t="n">
-        <v>75.59615384615384</v>
-      </c>
-      <c r="O14" t="n">
-        <v>81.45653846153846</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Danielle Mai</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>6</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>484.9</v>
-      </c>
-      <c r="G15" t="n">
-        <v>522.17</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>484.9</v>
-      </c>
-      <c r="M15" t="n">
-        <v>522.17</v>
-      </c>
-      <c r="N15" t="n">
-        <v>80.81666666666666</v>
-      </c>
-      <c r="O15" t="n">
-        <v>87.02833333333332</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Izzy Kruis</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>46</v>
-      </c>
-      <c r="C16" t="n">
-        <v>28</v>
-      </c>
-      <c r="D16" t="n">
-        <v>7</v>
-      </c>
-      <c r="E16" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2889.6</v>
-      </c>
-      <c r="G16" t="n">
-        <v>3113.63</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>2889.6</v>
-      </c>
-      <c r="M16" t="n">
-        <v>3113.63</v>
-      </c>
-      <c r="N16" t="n">
-        <v>62.81739130434782</v>
-      </c>
-      <c r="O16" t="n">
-        <v>67.68760869565217</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Jasmine Saiz</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>37</v>
-      </c>
-      <c r="C17" t="n">
-        <v>19</v>
-      </c>
-      <c r="D17" t="n">
-        <v>6</v>
-      </c>
-      <c r="E17" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F17" t="n">
-        <v>2391.46</v>
-      </c>
-      <c r="G17" t="n">
-        <v>2577.18</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="K17" t="n">
-        <v>22.09</v>
-      </c>
-      <c r="L17" t="n">
-        <v>2411.96</v>
-      </c>
-      <c r="M17" t="n">
-        <v>2599.27</v>
-      </c>
-      <c r="N17" t="n">
-        <v>65.18810810810811</v>
-      </c>
-      <c r="O17" t="n">
-        <v>70.25054054054054</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Justyne Martinez </t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>32</v>
-      </c>
-      <c r="C18" t="n">
-        <v>26</v>
-      </c>
-      <c r="D18" t="n">
-        <v>4</v>
-      </c>
-      <c r="E18" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F18" t="n">
-        <v>2149.7</v>
-      </c>
-      <c r="G18" t="n">
-        <v>2315.43</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>20</v>
-      </c>
-      <c r="K18" t="n">
-        <v>21.54</v>
-      </c>
-      <c r="L18" t="n">
-        <v>2169.7</v>
-      </c>
-      <c r="M18" t="n">
-        <v>2336.97</v>
-      </c>
-      <c r="N18" t="n">
-        <v>67.80312499999999</v>
-      </c>
-      <c r="O18" t="n">
-        <v>73.03031249999999</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Karen Trevizo</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>22</v>
-      </c>
-      <c r="C19" t="n">
-        <v>19</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1508.7</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1624.88</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1508.7</v>
-      </c>
-      <c r="M19" t="n">
-        <v>1624.88</v>
-      </c>
-      <c r="N19" t="n">
-        <v>68.57727272727271</v>
-      </c>
-      <c r="O19" t="n">
-        <v>73.85818181818182</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Krisdee Martinez</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>30</v>
-      </c>
-      <c r="C20" t="n">
-        <v>22</v>
-      </c>
-      <c r="D20" t="n">
-        <v>3</v>
-      </c>
-      <c r="E20" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2141.25</v>
-      </c>
-      <c r="G20" t="n">
-        <v>2307.68</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
-        <v>5</v>
-      </c>
-      <c r="K20" t="n">
-        <v>5.39</v>
-      </c>
-      <c r="L20" t="n">
-        <v>2146.25</v>
-      </c>
-      <c r="M20" t="n">
-        <v>2313.07</v>
-      </c>
-      <c r="N20" t="n">
-        <v>71.54166666666667</v>
-      </c>
-      <c r="O20" t="n">
-        <v>77.10233333333333</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Maggie  Farrell</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>26</v>
-      </c>
-      <c r="C21" t="n">
-        <v>17</v>
-      </c>
-      <c r="D21" t="n">
-        <v>3</v>
-      </c>
-      <c r="E21" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1740.3</v>
-      </c>
-      <c r="G21" t="n">
-        <v>1874.05</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="n">
-        <v>46</v>
-      </c>
-      <c r="K21" t="n">
-        <v>49.53</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1786.3</v>
-      </c>
-      <c r="M21" t="n">
-        <v>1923.58</v>
-      </c>
-      <c r="N21" t="n">
-        <v>68.70384615384616</v>
-      </c>
-      <c r="O21" t="n">
-        <v>73.98384615384614</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Makayla Baca</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>48</v>
-      </c>
-      <c r="C22" t="n">
-        <v>12</v>
-      </c>
-      <c r="D22" t="n">
-        <v>6</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F22" t="n">
-        <v>3852.42</v>
-      </c>
-      <c r="G22" t="n">
-        <v>4148.77</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
-        <v>28</v>
-      </c>
-      <c r="K22" t="n">
-        <v>30.16</v>
-      </c>
-      <c r="L22" t="n">
-        <v>3880.42</v>
-      </c>
-      <c r="M22" t="n">
-        <v>4178.93</v>
-      </c>
-      <c r="N22" t="n">
-        <v>80.84208333333333</v>
-      </c>
-      <c r="O22" t="n">
-        <v>87.06104166666667</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Vy Torino</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>37</v>
-      </c>
-      <c r="C23" t="n">
-        <v>22</v>
-      </c>
-      <c r="D23" t="n">
-        <v>9</v>
-      </c>
-      <c r="E23" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F23" t="n">
-        <v>2815.3</v>
-      </c>
-      <c r="G23" t="n">
-        <v>3031.7</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" t="n">
-        <v>5</v>
-      </c>
-      <c r="K23" t="n">
-        <v>5.38</v>
-      </c>
-      <c r="L23" t="n">
-        <v>2820.3</v>
-      </c>
-      <c r="M23" t="n">
-        <v>3037.08</v>
-      </c>
-      <c r="N23" t="n">
-        <v>76.22432432432433</v>
-      </c>
-      <c r="O23" t="n">
         <v>82.08324324324325</v>
       </c>
     </row>

</xml_diff>